<commit_message>
Estimates updated for Invoice and Yard pages
</commit_message>
<xml_diff>
--- a/TimeSheet-Kamran.xlsx
+++ b/TimeSheet-Kamran.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Task Name</t>
   </si>
@@ -56,6 +56,12 @@
   </si>
   <si>
     <t>TankHistory page</t>
+  </si>
+  <si>
+    <t>Yard page</t>
+  </si>
+  <si>
+    <t>Invoices page</t>
   </si>
 </sst>
 </file>
@@ -441,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="40.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -519,8 +525,33 @@
       <c r="G3">
         <v>9</v>
       </c>
+      <c r="H3">
+        <v>10</v>
+      </c>
       <c r="J3" s="3">
         <v>42121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="G4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="G5">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>